<commit_message>
Java 11 - Apache dependancy added
</commit_message>
<xml_diff>
--- a/src/test/resource/com/makemytrip/flightdetails/Flight Details.xlsx
+++ b/src/test/resource/com/makemytrip/flightdetails/Flight Details.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="96">
   <si>
     <t>Vistara</t>
   </si>
@@ -645,16 +645,16 @@
   <sheetData>
     <row r="2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -662,237 +662,237 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20">

</xml_diff>

<commit_message>
json cucumber report added in loaca
</commit_message>
<xml_diff>
--- a/src/test/resource/com/makemytrip/flightdetails/Flight Details.xlsx
+++ b/src/test/resource/com/makemytrip/flightdetails/Flight Details.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="104">
   <si>
     <t>Vistara</t>
   </si>
@@ -303,6 +303,30 @@
   </si>
   <si>
     <t>04 h 40 m</t>
+  </si>
+  <si>
+    <t>₹ 8,248</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>04 h 35 m</t>
+  </si>
+  <si>
+    <t>₹ 9,036</t>
+  </si>
+  <si>
+    <t>14:00</t>
+  </si>
+  <si>
+    <t>05 h 20 m</t>
+  </si>
+  <si>
+    <t>₹ 12,609</t>
+  </si>
+  <si>
+    <t>₹ 13,981</t>
   </si>
 </sst>
 </file>
@@ -645,69 +669,69 @@
   <sheetData>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -718,10 +742,10 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -729,13 +753,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -743,13 +767,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -757,13 +781,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -774,10 +798,10 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
@@ -788,10 +812,10 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -802,7 +826,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -813,13 +837,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
         <v>14</v>
@@ -827,13 +851,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
@@ -841,13 +865,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
@@ -858,7 +882,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -869,13 +893,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
         <v>14</v>
@@ -883,13 +907,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
@@ -897,30 +921,30 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22">

</xml_diff>